<commit_message>
updated import journal entry(cheque and journal voucher)
</commit_message>
<xml_diff>
--- a/public/extra/edit_excel/Journal_Import Data.xlsx
+++ b/public/extra/edit_excel/Journal_Import Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Accounting\public\extra\edit_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Accounting_modified\public\extra\edit_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Journal Date</t>
   </si>
@@ -51,13 +51,28 @@
   </si>
   <si>
     <t>Journal No</t>
+  </si>
+  <si>
+    <t>Cheque No</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Journal Type</t>
+  </si>
+  <si>
+    <t>Cheque Voucher</t>
+  </si>
+  <si>
+    <t>Journal Voucher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,13 +80,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,13 +111,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -368,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,47 +411,79 @@
     <col min="1" max="24" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>ChartofAccounts!$I$2:$I$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="I2:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="I2" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -440,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added date deposited column in add new journal entry and import journal entry
</commit_message>
<xml_diff>
--- a/public/extra/edit_excel/Journal_Import Data.xlsx
+++ b/public/extra/edit_excel/Journal_Import Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Journal Date</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Journal Voucher</t>
+  </si>
+  <si>
+    <t>Date Deposited</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +414,7 @@
     <col min="1" max="24" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,6 +447,9 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated chart of account output, placed a string newline replacer
</commit_message>
<xml_diff>
--- a/public/extra/edit_excel/Journal_Import Data.xlsx
+++ b/public/extra/edit_excel/Journal_Import Data.xlsx
@@ -27,12 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Journal Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost Center # </t>
   </si>
   <si>
     <t>Account</t>
@@ -403,26 +400,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="24" width="30.7109375" customWidth="1"/>
+    <col min="1" max="23" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -437,7 +434,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
@@ -446,10 +443,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -461,7 +455,7 @@
           <x14:formula1>
             <xm:f>ChartofAccounts!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -481,12 +475,12 @@
   <sheetData>
     <row r="2" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>